<commit_message>
Done Nunit Prescription & Appoinment
</commit_message>
<xml_diff>
--- a/server/server.Tests/Report/WhiteBox_Appointment_Report.xlsx
+++ b/server/server.Tests/Report/WhiteBox_Appointment_Report.xlsx
@@ -55,7 +55,7 @@
     <x:t>Appointment</x:t>
   </x:si>
   <x:si>
-    <x:t>Kiểm tra khi AppointmentForm null</x:t>
+    <x:t>Kiểm tra khi bệnh nhân không điền form và gửi form</x:t>
   </x:si>
   <x:si>
     <x:t>Line 49: if (appointmentForm == null) -&gt; throw ErrorHandlingException(400)</x:t>
@@ -70,91 +70,94 @@
     <x:t>{"form":"null"}</x:t>
   </x:si>
   <x:si>
+    <x:t>{"statusCode":400,"response":{"errorMessage":"Dữ liệu sai!"}}</x:t>
+  </x:si>
+  <x:si>
     <x:t>{"statusCode":400,"response":{"errorMessage":"Dữ liệu không hợp lệ"}}</x:t>
   </x:si>
   <x:si>
+    <x:t>FAIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19.77ms</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DLK02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kiểm tra khi bệnh nhân không chọn chuyên khoa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Line 52: if (string.IsNullOrWhiteSpace(appointmentForm.Department)) -&gt; throw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bệnh nhân đã đăng nhập, form thiếu Department</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{"department":"","doctor":"LÊ ANH TIẾN","service":"Tẩy trắng răng"}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{"statusCode":404,"response":{"errorMessage":"Vui lòng chọn khoa"}}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{"statusCode":400,"response":{"errorMessage":"Vui lòng chọn khoa"}}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.70ms</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DLK03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kiểm tra điều kiện triệu chứng quá dài (&gt;500 ký tự)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Line 67: if (!IsNullOrWhiteSpace(Symptoms) &amp;&amp; Symptoms.Count() &gt; 500) -&gt; throw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Condition Coverage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bệnh nhân đã đăng nhập, Symptoms có 501 ký tự</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{"symptomsLength":501,"condition1":"NOT empty = TRUE","condition2":"&gt;500 = TRUE"}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{"statusCode":400,"response":{"errorMessage":"Triệu chứng quá dài"}}</x:t>
+  </x:si>
+  <x:si>
     <x:t>PASS</x:t>
   </x:si>
   <x:si>
-    <x:t>17.41ms</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DLK02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kiểm tra khi Department rỗng - FAIL CASE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Line 52: if (string.IsNullOrWhiteSpace(appointmentForm.Department)) -&gt; throw</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bệnh nhân đã đăng nhập, form thiếu Department</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"department":"","doctor":"LÊ ANH TIẾN","service":"Tẩy trắng răng"}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"statusCode":404,"response":{"errorMessage":"Vui lòng chọn khoa"}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"statusCode":400,"response":{"errorMessage":"Vui lòng chọn khoa"}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FAIL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.67ms</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DLK03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kiểm tra điều kiện Symptoms quá dài (&gt;500 ký tự)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Line 67: if (!IsNullOrWhiteSpace(Symptoms) &amp;&amp; Symptoms.Count() &gt; 500) -&gt; throw</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Condition Coverage</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bệnh nhân đã đăng nhập, Symptoms có 501 ký tự</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"symptomsLength":501,"condition1":"NOT empty = TRUE","condition2":"&gt;500 = TRUE"}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"statusCode":400,"response":{"errorMessage":"Triệu chứng quá dài"}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0.91ms</x:t>
+    <x:t>0.92ms</x:t>
   </x:si>
   <x:si>
     <x:t>DLK04</x:t>
   </x:si>
   <x:si>
-    <x:t>Kiểm tra khi Specialty không tồn tại trong database - FAIL CASE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Line 74: GetSpecialty(Department) ?? throw ErrorHandlingException(404)</x:t>
+    <x:t>Kiểm tra khi không tìm thấy bác sĩ sau khi đã validate form và chuyên khoa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Line 77: if (doctor == null) -&gt; throw ErrorHandlingException(404, 'Không tìm thấy bác sĩ')</x:t>
   </x:si>
   <x:si>
     <x:t>Path Coverage</x:t>
   </x:si>
   <x:si>
-    <x:t>Bệnh nhân đã đăng nhập, form hợp lệ, Specialty không tồn tại</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"department":"Khoa Răng - Hàm - Mặt","specialtyExists":false}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"statusCode":404,"response":{"errorMessage":"Khoa không tồn tại trong hệ thống"}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"statusCode":404,"response":{"errorMessage":"Không tìm thấy khoa"}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9.25ms</x:t>
+    <x:t>Bệnh nhân đã đăng nhập, form hợp lệ, Specialty tồn tại, Doctor KHÔNG tồn tại</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{"department":"Khoa Răng - Hàm - Mặt","doctor":"LÊ ANH TIẾN"}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{"statusCode":404,"response":{"errorMessage":"Bác sĩ không tồn tại"}}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{"statusCode":404,"response":{"errorMessage":"Không tìm thấy bác sĩ"}}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13.36ms</x:t>
   </x:si>
   <x:si>
     <x:t>DLK05</x:t>
@@ -172,19 +175,19 @@
     <x:t>Bệnh nhân đã đăng nhập, form hợp lệ, ngày đặt = hôm nay</x:t>
   </x:si>
   <x:si>
-    <x:t>{"appointmentDate":"2026-01-01","diffDays":0,"condition":"diffDays &lt; 1 = TRUE"}</x:t>
+    <x:t>{"appointmentDate":"2026-01-02","diffDays":0,"condition":"diffDays &lt; 1 = TRUE"}</x:t>
   </x:si>
   <x:si>
     <x:t>{"statusCode":400,"response":{"errorMessage":"Vui lòng đặt lịch khám tối thiểu trước 1 ngày"}}</x:t>
   </x:si>
   <x:si>
-    <x:t>5.17ms</x:t>
+    <x:t>4.00ms</x:t>
   </x:si>
   <x:si>
     <x:t>DLK06</x:t>
   </x:si>
   <x:si>
-    <x:t>Kiểm tra ngày đặt lịch quá xa (diffDays &gt; 15) - FAIL CASE</x:t>
+    <x:t>Kiểm tra ngày đặt lịch quá xa (diffDays &gt; 15)E</x:t>
   </x:si>
   <x:si>
     <x:t>Line 97: if (diffDays &gt; 15) -&gt; throw ErrorHandlingException(400)</x:t>
@@ -193,7 +196,7 @@
     <x:t>Bệnh nhân đã đăng nhập, ngày đặt &gt; 15 ngày so với hôm nay</x:t>
   </x:si>
   <x:si>
-    <x:t>{"appointmentDate":"2026-01-21","diffDays":20,"condition":"diffDays &gt; 15 = TRUE"}</x:t>
+    <x:t>{"appointmentDate":"2026-01-22","diffDays":20,"condition":"diffDays &gt; 15 = TRUE"}</x:t>
   </x:si>
   <x:si>
     <x:t>{"statusCode":500,"response":{"errorMessage":"Ngày khám không được cách quá 15 ngày so với hôm nay"}}</x:t>
@@ -202,13 +205,10 @@
     <x:t>{"statusCode":400,"response":{"errorMessage":"Ngày khám không được cách quá 15 ngày so với hôm nay"}}</x:t>
   </x:si>
   <x:si>
-    <x:t>0.81ms</x:t>
-  </x:si>
-  <x:si>
     <x:t>DLK07</x:t>
   </x:si>
   <x:si>
-    <x:t>Kiểm tra khi đã có lịch hẹn chưa hoàn thành</x:t>
+    <x:t>Kiểm tra khi có lịch hẹn chưa hoàn thành</x:t>
   </x:si>
   <x:si>
     <x:t>Line 104-112: if (isExistAppointment != null) -&gt; throw ErrorHandlingException(400)</x:t>
@@ -223,16 +223,16 @@
     <x:t>{"statusCode":400,"response":{"errorMessage":"Bạn chưa hoàn thành lịch hẹn *"}}</x:t>
   </x:si>
   <x:si>
-    <x:t>{"statusCode":400,"response":{"errorMessage":"Bạn chưa hoàn thành lịch hẹn 1/2/2026 Sáng"}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4.41ms</x:t>
+    <x:t>{"statusCode":400,"response":{"errorMessage":"Bạn chưa hoàn thành lịch hẹn 1/3/2026 Sáng"}}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4.61ms</x:t>
   </x:si>
   <x:si>
     <x:t>DLK08</x:t>
   </x:si>
   <x:si>
-    <x:t>Kiểm tra khi slot đã đầy (&gt;15 lịch hẹn) - trả về các slot khả dụng</x:t>
+    <x:t>Kiểm tra khi slot đã đầy (&gt;15 lịch hẹn)</x:t>
   </x:si>
   <x:si>
     <x:t>Line 119-128: if (quantityAppointment &gt; 15) -&gt; return Ok(availableAppointments)</x:t>
@@ -244,19 +244,19 @@
     <x:t>{"slotCount":16,"condition":"quantityAppointment &gt; 15 = TRUE"}</x:t>
   </x:si>
   <x:si>
-    <x:t>{"statusCode":200,"response":{"availableAppointments":"List of available slots"}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"statusCode":200,"response":{"availableAppointments":[{"Date":"2026-01-05T22:07:11.6745479+07:00","Time":"Chiều"},{"Date":"2026-01-06T22:07:11.6746069+07:00","Time":"Sáng"}]}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.79ms</x:t>
+    <x:t>{"statusCode":200,"response":{"availableAppointments":"*"}}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{"statusCode":200,"response":{"availableAppointments":[{"Date":"2026-01-06T00:10:37.1293944+07:00","Time":"Chiều"},{"Date":"2026-01-07T00:10:37.12943+07:00","Time":"Sáng"}]}}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.19ms</x:t>
   </x:si>
   <x:si>
     <x:t>DLK09</x:t>
   </x:si>
   <x:si>
-    <x:t>Đặt lịch thành công - Full Path Coverage</x:t>
+    <x:t>Đặt lịch thành công</x:t>
   </x:si>
   <x:si>
     <x:t>Line 130-139: All validations pass -&gt; Appointment() -&gt; return Ok('Đặt lịch thành công!')</x:t>
@@ -268,13 +268,13 @@
     <x:t>Bệnh nhân đã đăng nhập, tất cả dữ liệu hợp lệ, slot còn trống</x:t>
   </x:si>
   <x:si>
-    <x:t>{"department":"Khoa Răng - Hàm - Mặt","doctor":"LÊ ANH TIẾN","service":"Tẩy trắng răng","date":"2026-01-04","time":"Sáng"}</x:t>
+    <x:t>{"department":"Khoa Răng - Hàm - Mặt","doctor":"LÊ ANH TIẾN","service":"Tẩy trắng răng","date":"2026-01-05","time":"Sáng"}</x:t>
   </x:si>
   <x:si>
     <x:t>{"statusCode":200,"response":{"message":"Đặt lịch thành công!"}}</x:t>
   </x:si>
   <x:si>
-    <x:t>3.56ms</x:t>
+    <x:t>3.29ms</x:t>
   </x:si>
   <x:si>
     <x:t>DLK10</x:t>
@@ -283,7 +283,7 @@
     <x:t>UpdateAppointmentStatus</x:t>
   </x:si>
   <x:si>
-    <x:t>Kiểm tra bác sĩ không có quyền cập nhật status khác 'Đã khám' - FAIL CASE</x:t>
+    <x:t>Kiểm tra bác sĩ không có quyền cập nhật status khác 'Đã khám'</x:t>
   </x:si>
   <x:si>
     <x:t>Line 185-189: if (role == 'doctor' &amp;&amp; status != 'Đã khám') -&gt; throw 403</x:t>
@@ -301,7 +301,7 @@
     <x:t>{"statusCode":403,"response":{"errorMessage":"Bạn không có quyền!"}}</x:t>
   </x:si>
   <x:si>
-    <x:t>1.93ms</x:t>
+    <x:t>1.56ms</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -331,7 +331,7 @@
       <x:b/>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
-      <x:color rgb="FF008000"/>
+      <x:color rgb="FFFF0000"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
     </x:font>
@@ -339,7 +339,7 @@
       <x:b/>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
-      <x:color rgb="FFFF0000"/>
+      <x:color rgb="FF008000"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
     </x:font>
@@ -358,12 +358,12 @@
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor rgb="FF90EE90"/>
+        <x:fgColor rgb="FFFFB6C1"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor rgb="FFFFB6C1"/>
+        <x:fgColor rgb="FF90EE90"/>
       </x:patternFill>
     </x:fill>
   </x:fills>
@@ -817,45 +817,45 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="I2" s="2" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="J2" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="K2" s="2" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:11">
       <x:c r="A3" s="2" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B3" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="C3" s="2" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D3" s="2" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="E3" s="2" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="F3" s="2" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G3" s="2" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H3" s="2" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="I3" s="2" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="J3" s="4" t="s">
         <x:v>28</x:v>
+      </x:c>
+      <x:c r="J3" s="3" t="s">
+        <x:v>20</x:v>
       </x:c>
       <x:c r="K3" s="2" t="s">
         <x:v>29</x:v>
@@ -889,116 +889,116 @@
       <x:c r="I4" s="2" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="J4" s="3" t="s">
-        <x:v>19</x:v>
+      <x:c r="J4" s="4" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="K4" s="2" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:11">
       <x:c r="A5" s="2" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B5" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="C5" s="2" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="D5" s="2" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E5" s="2" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="F5" s="2" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G5" s="2" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="H5" s="2" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="I5" s="2" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="J5" s="4" t="s">
-        <x:v>28</x:v>
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="J5" s="3" t="s">
+        <x:v>20</x:v>
       </x:c>
       <x:c r="K5" s="2" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:11">
       <x:c r="A6" s="2" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B6" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="D6" s="2" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E6" s="2" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F6" s="2" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="G6" s="2" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="H6" s="2" t="s">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="I6" s="2" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="J6" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="J6" s="4" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="K6" s="2" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:11">
       <x:c r="A7" s="2" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B7" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="C7" s="2" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D7" s="2" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E7" s="2" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="F7" s="2" t="s">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="G7" s="2" t="s">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="H7" s="2" t="s">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="I7" s="2" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="J7" s="4" t="s">
-        <x:v>28</x:v>
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="J7" s="3" t="s">
+        <x:v>20</x:v>
       </x:c>
       <x:c r="K7" s="2" t="s">
-        <x:v>62</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:11">
@@ -1015,7 +1015,7 @@
         <x:v>65</x:v>
       </x:c>
       <x:c r="E8" s="2" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="F8" s="2" t="s">
         <x:v>66</x:v>
@@ -1029,8 +1029,8 @@
       <x:c r="I8" s="2" t="s">
         <x:v>69</x:v>
       </x:c>
-      <x:c r="J8" s="3" t="s">
-        <x:v>19</x:v>
+      <x:c r="J8" s="4" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="K8" s="2" t="s">
         <x:v>70</x:v>
@@ -1065,7 +1065,7 @@
         <x:v>77</x:v>
       </x:c>
       <x:c r="J9" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="K9" s="2" t="s">
         <x:v>78</x:v>
@@ -1099,8 +1099,8 @@
       <x:c r="I10" s="2" t="s">
         <x:v>85</x:v>
       </x:c>
-      <x:c r="J10" s="3" t="s">
-        <x:v>19</x:v>
+      <x:c r="J10" s="4" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="K10" s="2" t="s">
         <x:v>86</x:v>
@@ -1120,7 +1120,7 @@
         <x:v>90</x:v>
       </x:c>
       <x:c r="E11" s="2" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F11" s="2" t="s">
         <x:v>91</x:v>
@@ -1134,8 +1134,8 @@
       <x:c r="I11" s="2" t="s">
         <x:v>94</x:v>
       </x:c>
-      <x:c r="J11" s="4" t="s">
-        <x:v>28</x:v>
+      <x:c r="J11" s="3" t="s">
+        <x:v>20</x:v>
       </x:c>
       <x:c r="K11" s="2" t="s">
         <x:v>95</x:v>

</xml_diff>